<commit_message>
correct for different time formats
</commit_message>
<xml_diff>
--- a/data/spuibeheer/extern/verwerkt_in_excel/os_KGO_2023.xlsx
+++ b/data/spuibeheer/extern/verwerkt_in_excel/os_KGO_2023.xlsx
@@ -340,10 +340,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="3">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="d/mm/yy;@"/>
     <numFmt numFmtId="165" formatCode="h:mm;@"/>
-    <numFmt numFmtId="166" formatCode="dd\-mm\-yy;@"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -562,9 +561,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -612,6 +608,7 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -892,10 +889,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H117"/>
+  <dimension ref="A1:G117"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A110" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D88" sqref="D88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -903,8 +900,8 @@
     <col min="1" max="1" width="10.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="20" t="s">
+    <row r="1" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="19" t="s">
         <v>97</v>
       </c>
       <c r="B1" s="1" t="s">
@@ -914,7 +911,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>44986</v>
       </c>
@@ -925,7 +922,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>44987</v>
       </c>
@@ -936,7 +933,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>44988</v>
       </c>
@@ -947,7 +944,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>44989</v>
       </c>
@@ -958,7 +955,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>44990</v>
       </c>
@@ -969,7 +966,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>44991</v>
       </c>
@@ -980,7 +977,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>44992</v>
       </c>
@@ -991,7 +988,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>44993</v>
       </c>
@@ -1002,19 +999,19 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="10" t="s">
+    <row r="10" spans="1:7" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="C10" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="H10" s="16"/>
-    </row>
-    <row r="11" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B10" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="G10" s="15"/>
+    </row>
+    <row r="11" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>44995</v>
       </c>
@@ -1025,7 +1022,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>44996</v>
       </c>
@@ -1036,7 +1033,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
         <v>44997</v>
       </c>
@@ -1047,7 +1044,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
         <v>44998</v>
       </c>
@@ -1058,7 +1055,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
         <v>44999</v>
       </c>
@@ -1069,7 +1066,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:7" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
         <v>45000</v>
       </c>
@@ -1080,7 +1077,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
         <v>45001</v>
       </c>
@@ -1091,7 +1088,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="2">
         <v>45002</v>
       </c>
@@ -1102,7 +1099,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A19" s="2">
         <v>45003</v>
       </c>
@@ -1113,7 +1110,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" s="2">
         <v>45004</v>
       </c>
@@ -1124,7 +1121,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A21" s="2">
         <v>45005</v>
       </c>
@@ -1135,7 +1132,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A22" s="2">
         <v>45006</v>
       </c>
@@ -1146,7 +1143,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A23" s="2">
         <v>45007</v>
       </c>
@@ -1157,7 +1154,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A24" s="2">
         <v>45008</v>
       </c>
@@ -1168,7 +1165,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A25" s="2">
         <v>45009</v>
       </c>
@@ -1179,18 +1176,18 @@
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A26" s="2">
         <v>45010</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="C26" s="6" t="s">
+      <c r="C26" s="5" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="27" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A27" s="2">
         <v>45011</v>
       </c>
@@ -1201,7 +1198,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="28" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A28" s="2">
         <v>45012</v>
       </c>
@@ -1212,7 +1209,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="29" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A29" s="2">
         <v>45013</v>
       </c>
@@ -1223,7 +1220,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="30" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A30" s="2">
         <v>45014</v>
       </c>
@@ -1234,7 +1231,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A31" s="2">
         <v>45015</v>
       </c>
@@ -1245,36 +1242,36 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A32" s="17">
+    <row r="32" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A32" s="16">
         <v>45017</v>
       </c>
-      <c r="B32" s="18" t="s">
+      <c r="B32" s="17" t="s">
         <v>78</v>
       </c>
-      <c r="C32" s="18" t="s">
+      <c r="C32" s="17" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="33" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="17">
+    <row r="33" spans="1:3" s="10" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A33" s="16">
         <v>45018</v>
       </c>
-      <c r="B33" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="C33" s="18" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" s="11" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A34" s="9">
+      <c r="B33" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C33" s="17" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A34" s="8">
         <v>45019</v>
       </c>
-      <c r="B34" s="7" t="s">
+      <c r="B34" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="C34" s="7" t="s">
+      <c r="C34" s="6" t="s">
         <v>16</v>
       </c>
     </row>
@@ -1367,13 +1364,13 @@
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A43" s="10" t="s">
+      <c r="A43" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B43" s="14" t="s">
-        <v>0</v>
-      </c>
-      <c r="C43" s="15" t="s">
+      <c r="B43" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C43" s="14" t="s">
         <v>0</v>
       </c>
     </row>
@@ -1436,7 +1433,7 @@
       <c r="A49" s="2">
         <v>45000</v>
       </c>
-      <c r="B49" s="12" t="s">
+      <c r="B49" s="11" t="s">
         <v>0</v>
       </c>
       <c r="C49" s="4" t="s">
@@ -1609,54 +1606,54 @@
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A65" s="17">
+      <c r="A65" s="16">
         <v>45017</v>
       </c>
-      <c r="B65" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="C65" s="19" t="s">
+      <c r="B65" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C65" s="18" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A66" s="17">
+      <c r="A66" s="16">
         <v>45018</v>
       </c>
-      <c r="B66" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="C66" s="19" t="s">
+      <c r="B66" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C66" s="18" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="67" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A67" s="9">
+      <c r="A67" s="8">
         <v>45019</v>
       </c>
-      <c r="B67" s="7" t="s">
+      <c r="B67" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C67" s="8" t="s">
+      <c r="C67" s="7" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A68" s="5">
+      <c r="A68" s="20">
         <v>45020</v>
       </c>
       <c r="B68" s="3"/>
       <c r="C68" s="3"/>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A69" s="5">
+      <c r="A69" s="20">
         <v>45021</v>
       </c>
       <c r="B69" s="3"/>
       <c r="C69" s="3"/>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A70" s="5">
+      <c r="A70" s="20">
         <v>45022</v>
       </c>
       <c r="B70" s="3" t="s">
@@ -1667,7 +1664,7 @@
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A71" s="5">
+      <c r="A71" s="20">
         <v>45023</v>
       </c>
       <c r="B71" s="3" t="s">
@@ -1678,7 +1675,7 @@
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A72" s="5">
+      <c r="A72" s="20">
         <v>45024</v>
       </c>
       <c r="B72" s="3" t="s">
@@ -1689,7 +1686,7 @@
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A73" s="5">
+      <c r="A73" s="20">
         <v>45025</v>
       </c>
       <c r="B73" s="3" t="s">
@@ -1700,7 +1697,7 @@
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A74" s="5">
+      <c r="A74" s="20">
         <v>45026</v>
       </c>
       <c r="B74" s="3" t="s">
@@ -1711,7 +1708,7 @@
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A75" s="5">
+      <c r="A75" s="20">
         <v>45027</v>
       </c>
       <c r="B75" s="3" t="s">
@@ -1722,7 +1719,7 @@
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A76" s="5">
+      <c r="A76" s="20">
         <v>45028</v>
       </c>
       <c r="B76" s="3" t="s">
@@ -1733,7 +1730,7 @@
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A77" s="5">
+      <c r="A77" s="20">
         <v>45029</v>
       </c>
       <c r="B77" s="3" t="s">
@@ -1744,7 +1741,7 @@
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A78" s="5">
+      <c r="A78" s="20">
         <v>45030</v>
       </c>
       <c r="B78" s="3" t="s">
@@ -1755,7 +1752,7 @@
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A79" s="5">
+      <c r="A79" s="20">
         <v>45031</v>
       </c>
       <c r="B79" s="3" t="s">
@@ -1766,7 +1763,7 @@
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A80" s="5">
+      <c r="A80" s="20">
         <v>45032</v>
       </c>
       <c r="B80" s="3" t="s">
@@ -1777,7 +1774,7 @@
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A81" s="5">
+      <c r="A81" s="20">
         <v>45033</v>
       </c>
       <c r="B81" s="3" t="s">
@@ -1788,7 +1785,7 @@
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A82" s="5">
+      <c r="A82" s="20">
         <v>45034</v>
       </c>
       <c r="B82" s="3" t="s">
@@ -1799,7 +1796,7 @@
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A83" s="5">
+      <c r="A83" s="20">
         <v>45035</v>
       </c>
       <c r="B83" s="3" t="s">
@@ -1810,7 +1807,7 @@
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A84" s="5">
+      <c r="A84" s="20">
         <v>45036</v>
       </c>
       <c r="B84" s="3" t="s">
@@ -1821,7 +1818,7 @@
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A85" s="5">
+      <c r="A85" s="20">
         <v>45037</v>
       </c>
       <c r="B85" s="3" t="s">
@@ -1832,7 +1829,7 @@
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A86" s="5">
+      <c r="A86" s="20">
         <v>45038</v>
       </c>
       <c r="B86" s="3" t="s">
@@ -1843,7 +1840,7 @@
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A87" s="5">
+      <c r="A87" s="20">
         <v>45039</v>
       </c>
       <c r="B87" s="3" t="s">
@@ -1854,7 +1851,7 @@
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A88" s="5">
+      <c r="A88" s="20">
         <v>45040</v>
       </c>
       <c r="B88" s="3" t="s">
@@ -1865,7 +1862,7 @@
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A89" s="5">
+      <c r="A89" s="20">
         <v>45041</v>
       </c>
       <c r="B89" s="3" t="s">
@@ -1876,7 +1873,7 @@
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A90" s="5">
+      <c r="A90" s="20">
         <v>45042</v>
       </c>
       <c r="B90" s="3" t="s">
@@ -1887,7 +1884,7 @@
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A91" s="5">
+      <c r="A91" s="20">
         <v>45043</v>
       </c>
       <c r="B91" s="3" t="s">
@@ -1898,7 +1895,7 @@
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A92" s="5">
+      <c r="A92" s="20">
         <v>45050</v>
       </c>
       <c r="B92" s="3" t="s">
@@ -1909,7 +1906,7 @@
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A93" s="5">
+      <c r="A93" s="20">
         <v>45020</v>
       </c>
       <c r="B93" s="3" t="s">
@@ -1920,7 +1917,7 @@
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A94" s="5">
+      <c r="A94" s="20">
         <v>45021</v>
       </c>
       <c r="B94" s="3" t="s">
@@ -1931,7 +1928,7 @@
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A95" s="5">
+      <c r="A95" s="20">
         <v>45022</v>
       </c>
       <c r="B95" s="3" t="s">
@@ -1942,7 +1939,7 @@
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A96" s="5">
+      <c r="A96" s="20">
         <v>45023</v>
       </c>
       <c r="B96" s="3" t="s">
@@ -1953,7 +1950,7 @@
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A97" s="5">
+      <c r="A97" s="20">
         <v>45024</v>
       </c>
       <c r="B97" s="3" t="s">
@@ -1964,7 +1961,7 @@
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A98" s="5">
+      <c r="A98" s="20">
         <v>45025</v>
       </c>
       <c r="B98" s="3" t="s">
@@ -1975,7 +1972,7 @@
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A99" s="5">
+      <c r="A99" s="20">
         <v>45026</v>
       </c>
       <c r="B99" s="3" t="s">
@@ -1986,7 +1983,7 @@
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A100" s="5">
+      <c r="A100" s="20">
         <v>45027</v>
       </c>
       <c r="B100" s="3" t="s">
@@ -1997,7 +1994,7 @@
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A101" s="5">
+      <c r="A101" s="20">
         <v>45028</v>
       </c>
       <c r="B101" s="3" t="s">
@@ -2008,7 +2005,7 @@
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A102" s="5">
+      <c r="A102" s="20">
         <v>45029</v>
       </c>
       <c r="B102" s="3" t="s">
@@ -2019,7 +2016,7 @@
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A103" s="5">
+      <c r="A103" s="20">
         <v>45030</v>
       </c>
       <c r="B103" s="3" t="s">
@@ -2030,7 +2027,7 @@
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A104" s="5">
+      <c r="A104" s="20">
         <v>45031</v>
       </c>
       <c r="B104" s="3" t="s">
@@ -2041,7 +2038,7 @@
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A105" s="5">
+      <c r="A105" s="20">
         <v>45032</v>
       </c>
       <c r="B105" s="3" t="s">
@@ -2052,7 +2049,7 @@
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A106" s="5">
+      <c r="A106" s="20">
         <v>45033</v>
       </c>
       <c r="B106" s="3" t="s">
@@ -2063,14 +2060,14 @@
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A107" s="5">
+      <c r="A107" s="20">
         <v>45034</v>
       </c>
       <c r="B107" s="3"/>
       <c r="C107" s="4"/>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A108" s="5">
+      <c r="A108" s="20">
         <v>45035</v>
       </c>
       <c r="B108" s="3" t="s">
@@ -2081,18 +2078,18 @@
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A109" s="5">
+      <c r="A109" s="20">
         <v>45036</v>
       </c>
-      <c r="B109" s="12" t="s">
+      <c r="B109" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="C109" s="13" t="s">
+      <c r="C109" s="12" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A110" s="5">
+      <c r="A110" s="20">
         <v>45037</v>
       </c>
       <c r="B110" s="3" t="s">
@@ -2103,7 +2100,7 @@
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A111" s="5">
+      <c r="A111" s="20">
         <v>45038</v>
       </c>
       <c r="B111" s="3" t="s">
@@ -2114,7 +2111,7 @@
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A112" s="5">
+      <c r="A112" s="20">
         <v>45039</v>
       </c>
       <c r="B112" s="3" t="s">
@@ -2125,7 +2122,7 @@
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A113" s="5">
+      <c r="A113" s="20">
         <v>45040</v>
       </c>
       <c r="B113" s="3" t="s">
@@ -2136,7 +2133,7 @@
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A114" s="5">
+      <c r="A114" s="20">
         <v>45041</v>
       </c>
       <c r="B114" s="3" t="s">
@@ -2147,7 +2144,7 @@
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A115" s="5">
+      <c r="A115" s="20">
         <v>45042</v>
       </c>
       <c r="B115" s="3" t="s">
@@ -2158,14 +2155,14 @@
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A116" s="5">
+      <c r="A116" s="20">
         <v>45043</v>
       </c>
       <c r="B116" s="3"/>
       <c r="C116" s="4"/>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A117" s="5">
+      <c r="A117" s="20">
         <v>45050</v>
       </c>
       <c r="B117" s="3"/>

</xml_diff>